<commit_message>
new powerpoints, modified work bd given current state, added draft for possible change order
</commit_message>
<xml_diff>
--- a/work breakdown.xlsx
+++ b/work breakdown.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason Wu\Desktop\College work\sdg\sdg-database-migration-documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D2D588-8833-4A40-99BB-B8668404A402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F9C9D3-2458-48AD-B55D-A7729F4142C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{7FD9875C-3BD0-4C00-9D64-EBFC33032F5D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
   <si>
     <t>Task number</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>Set up login/logout management</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
   </si>
 </sst>
 </file>
@@ -484,7 +487,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +496,7 @@
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
     <col min="3" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
     <col min="7" max="7" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -562,7 +565,7 @@
         <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
@@ -586,7 +589,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
         <v>7</v>
@@ -610,7 +613,7 @@
         <v>25</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
@@ -634,7 +637,7 @@
         <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
         <v>7</v>
@@ -658,7 +661,7 @@
         <v>44</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
@@ -706,7 +709,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G9" t="s">
         <v>7</v>
@@ -730,7 +733,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G10" t="s">
         <v>7</v>
@@ -819,11 +822,11 @@
         <v>44629</v>
       </c>
       <c r="D14" s="1">
-        <v>44705</v>
+        <v>44699</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>26</v>
@@ -843,11 +846,11 @@
         <v>44673</v>
       </c>
       <c r="D15" s="1">
-        <v>44694</v>
+        <v>44699</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>28</v>
@@ -891,11 +894,11 @@
         <v>44629</v>
       </c>
       <c r="D17" s="1">
-        <v>44705</v>
+        <v>44699</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="0"/>
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>26</v>
@@ -915,11 +918,11 @@
         <v>44629</v>
       </c>
       <c r="D18" s="1">
-        <v>44705</v>
+        <v>44699</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="0"/>
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>26</v>
@@ -936,16 +939,18 @@
         <v>23</v>
       </c>
       <c r="C19" s="1">
-        <v>44694</v>
+        <v>44695</v>
       </c>
       <c r="D19" s="1">
-        <v>44705</v>
+        <v>44699</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="F19" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G19" t="s">
         <v>7</v>
       </c>

</xml_diff>